<commit_message>
Pulled in interfaces chapter. Updated bill of materials.
</commit_message>
<xml_diff>
--- a/doc/design/bill_of_materials.xlsx
+++ b/doc/design/bill_of_materials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="49">
   <si>
     <t>D-H Transformation Block</t>
   </si>
@@ -151,6 +151,21 @@
   </si>
   <si>
     <t>Sine Cosine</t>
+  </si>
+  <si>
+    <t>Hz</t>
+  </si>
+  <si>
+    <t>sec</t>
+  </si>
+  <si>
+    <t>Jacobian Block</t>
+  </si>
+  <si>
+    <t>addition</t>
+  </si>
+  <si>
+    <t>subtraction</t>
   </si>
 </sst>
 </file>
@@ -204,7 +219,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -227,6 +242,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -311,7 +363,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -336,6 +388,19 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="81">
@@ -748,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M54"/>
+  <dimension ref="A2:M62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="B35" sqref="B35:M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0"/>
@@ -801,103 +866,59 @@
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:13" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="6">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="6">
-        <v>3</v>
-      </c>
-      <c r="G4" s="6">
-        <v>645</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0</v>
-      </c>
-      <c r="I4" s="6">
-        <v>146</v>
-      </c>
-      <c r="J4" s="6">
-        <v>151</v>
-      </c>
-      <c r="K4" s="6">
-        <v>0</v>
-      </c>
-      <c r="L4" s="6">
-        <v>0</v>
-      </c>
-      <c r="M4" s="6">
-        <v>0</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
     </row>
     <row r="5" spans="1:13" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="6">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="6">
-        <v>3</v>
-      </c>
-      <c r="G5" s="6">
-        <v>645</v>
-      </c>
-      <c r="H5" s="6">
-        <v>2</v>
-      </c>
-      <c r="I5" s="6">
-        <v>294</v>
-      </c>
-      <c r="J5" s="6">
-        <v>274</v>
-      </c>
-      <c r="K5" s="6">
-        <v>0</v>
-      </c>
-      <c r="L5" s="6">
-        <v>2</v>
-      </c>
-      <c r="M5" s="6">
-        <v>0</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" spans="1:13" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="10" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C6" s="6">
         <v>1</v>
@@ -906,104 +927,116 @@
         <v>28</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F6" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G6" s="6">
-        <v>267</v>
+        <v>645</v>
       </c>
       <c r="H6" s="6">
         <v>0</v>
       </c>
       <c r="I6" s="6">
+        <v>146</v>
+      </c>
+      <c r="J6" s="6">
+        <v>151</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A7" s="3"/>
+      <c r="B7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="6">
+        <v>3</v>
+      </c>
+      <c r="G7" s="6">
+        <v>645</v>
+      </c>
+      <c r="H7" s="6">
+        <v>2</v>
+      </c>
+      <c r="I7" s="6">
+        <v>294</v>
+      </c>
+      <c r="J7" s="6">
+        <v>274</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0</v>
+      </c>
+      <c r="L7" s="6">
+        <v>2</v>
+      </c>
+      <c r="M7" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A8" s="3"/>
+      <c r="B8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="6">
+        <v>5</v>
+      </c>
+      <c r="G8" s="6">
+        <v>267</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0</v>
+      </c>
+      <c r="I8" s="6">
         <f>131+94</f>
         <v>225</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J8" s="6">
         <v>0</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K8" s="6">
         <v>0</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L8" s="6">
         <v>0</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M8" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="27" hidden="1" customHeight="1">
-      <c r="A7" s="5"/>
-      <c r="B7" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="6">
-        <v>1</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="6">
-        <v>36</v>
-      </c>
-      <c r="G7" s="6">
-        <v>296.95999999999998</v>
-      </c>
-      <c r="H7" s="6">
-        <v>7</v>
-      </c>
-      <c r="I7" s="6">
-        <v>2697</v>
-      </c>
-      <c r="J7" s="6">
-        <v>4900</v>
-      </c>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" spans="1:13" ht="27" hidden="1" customHeight="1">
-      <c r="A8" s="5"/>
-      <c r="B8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="6">
-        <v>1</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="6">
-        <v>35</v>
-      </c>
-      <c r="G8" s="6">
-        <v>258.26</v>
-      </c>
-      <c r="H8" s="6">
-        <v>7</v>
-      </c>
-      <c r="I8" s="6">
-        <v>2631</v>
-      </c>
-      <c r="J8" s="6">
-        <v>3632</v>
-      </c>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
     </row>
     <row r="9" spans="1:13" ht="27" hidden="1" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="4" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C9" s="6">
         <v>1</v>
@@ -1015,19 +1048,19 @@
         <v>13</v>
       </c>
       <c r="F9" s="6">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="G9" s="6">
-        <v>303</v>
+        <v>296.95999999999998</v>
       </c>
       <c r="H9" s="6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I9" s="6">
-        <v>217</v>
+        <v>2697</v>
       </c>
       <c r="J9" s="6">
-        <v>469</v>
+        <v>4900</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
@@ -1036,7 +1069,7 @@
     <row r="10" spans="1:13" ht="27" hidden="1" customHeight="1">
       <c r="A10" s="5"/>
       <c r="B10" s="4" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C10" s="6">
         <v>1</v>
@@ -1048,19 +1081,19 @@
         <v>13</v>
       </c>
       <c r="F10" s="6">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="G10" s="6">
-        <v>223</v>
+        <v>258.26</v>
       </c>
       <c r="H10" s="6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I10" s="6">
-        <v>154</v>
+        <v>2631</v>
       </c>
       <c r="J10" s="6">
-        <v>166</v>
+        <v>3632</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -1084,16 +1117,16 @@
         <v>11</v>
       </c>
       <c r="G11" s="6">
-        <v>209</v>
+        <v>303</v>
       </c>
       <c r="H11" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="6">
-        <v>55</v>
+        <v>217</v>
       </c>
       <c r="J11" s="6">
-        <v>279</v>
+        <v>469</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -1102,7 +1135,7 @@
     <row r="12" spans="1:13" ht="27" hidden="1" customHeight="1">
       <c r="A12" s="5"/>
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C12" s="6">
         <v>1</v>
@@ -1113,20 +1146,20 @@
       <c r="E12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>22</v>
+      <c r="F12" s="6">
+        <v>5</v>
       </c>
       <c r="G12" s="6">
-        <v>414</v>
+        <v>223</v>
       </c>
       <c r="H12" s="6">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="I12" s="6">
-        <v>3698</v>
+        <v>154</v>
       </c>
       <c r="J12" s="6">
-        <v>0</v>
+        <v>166</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -1135,7 +1168,7 @@
     <row r="13" spans="1:13" ht="27" hidden="1" customHeight="1">
       <c r="A13" s="5"/>
       <c r="B13" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C13" s="6">
         <v>1</v>
@@ -1146,69 +1179,86 @@
       <c r="E13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>22</v>
+      <c r="F13" s="6">
+        <v>11</v>
       </c>
       <c r="G13" s="6">
-        <v>162</v>
+        <v>209</v>
       </c>
       <c r="H13" s="6">
-        <v>574</v>
+        <v>0</v>
       </c>
       <c r="I13" s="6">
-        <v>62872</v>
+        <v>55</v>
       </c>
       <c r="J13" s="6">
-        <v>0</v>
+        <v>279</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
     </row>
-    <row r="14" spans="1:13" ht="27" customHeight="1">
+    <row r="14" spans="1:13" ht="27" hidden="1" customHeight="1">
       <c r="A14" s="5"/>
-      <c r="B14" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-    </row>
-    <row r="15" spans="1:13" ht="27" customHeight="1">
+      <c r="B14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="6">
+        <v>414</v>
+      </c>
+      <c r="H14" s="6">
+        <v>32</v>
+      </c>
+      <c r="I14" s="6">
+        <v>3698</v>
+      </c>
+      <c r="J14" s="6">
+        <v>0</v>
+      </c>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="1:13" ht="27" hidden="1" customHeight="1">
       <c r="A15" s="5"/>
       <c r="B15" s="4" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C15" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+        <v>13</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="6">
+        <v>162</v>
+      </c>
       <c r="H15" s="6">
-        <f>$C15*H$4</f>
+        <v>574</v>
+      </c>
+      <c r="I15" s="6">
+        <v>62872</v>
+      </c>
+      <c r="J15" s="6">
         <v>0</v>
-      </c>
-      <c r="I15" s="6">
-        <f>$C15*I$4</f>
-        <v>292</v>
-      </c>
-      <c r="J15" s="6">
-        <f>$C15*J$4</f>
-        <v>302</v>
       </c>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
@@ -1216,43 +1266,28 @@
     </row>
     <row r="16" spans="1:13" ht="27" customHeight="1">
       <c r="A16" s="5"/>
-      <c r="B16" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="6">
-        <v>2</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6">
-        <f>$C16*H$5</f>
-        <v>4</v>
-      </c>
-      <c r="I16" s="6">
-        <f t="shared" ref="I16:J16" si="0">$C16*I$5</f>
-        <v>588</v>
-      </c>
-      <c r="J16" s="6">
-        <f t="shared" si="0"/>
-        <v>548</v>
-      </c>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
+      <c r="B16" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
     </row>
     <row r="17" spans="1:13" ht="27" customHeight="1">
       <c r="A17" s="5"/>
       <c r="B17" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C17" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>28</v>
@@ -1263,16 +1298,16 @@
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6">
-        <f>$C17*H$5</f>
-        <v>8</v>
+        <f>$C17*H$6</f>
+        <v>0</v>
       </c>
       <c r="I17" s="6">
-        <f>$C17*I$5</f>
-        <v>1176</v>
+        <f>$C17*I$6</f>
+        <v>292</v>
       </c>
       <c r="J17" s="6">
-        <f>$C17*J$5</f>
-        <v>1096</v>
+        <f>$C17*J$6</f>
+        <v>302</v>
       </c>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
@@ -1280,8 +1315,8 @@
     </row>
     <row r="18" spans="1:13" ht="27" customHeight="1">
       <c r="A18" s="5"/>
-      <c r="B18" s="8" t="s">
-        <v>8</v>
+      <c r="B18" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="C18" s="6">
         <v>1</v>
@@ -1292,21 +1327,19 @@
       <c r="E18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="6">
-        <v>12</v>
-      </c>
+      <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6">
-        <f>SUM(H15:H17)</f>
-        <v>12</v>
+        <f>$C18*H$7</f>
+        <v>2</v>
       </c>
       <c r="I18" s="6">
-        <f t="shared" ref="I18:J18" si="1">SUM(I15:I17)</f>
-        <v>2056</v>
+        <f t="shared" ref="I18:J18" si="0">$C18*I$7</f>
+        <v>294</v>
       </c>
       <c r="J18" s="6">
-        <f t="shared" si="1"/>
-        <v>1946</v>
+        <f t="shared" si="0"/>
+        <v>274</v>
       </c>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
@@ -1314,28 +1347,43 @@
     </row>
     <row r="19" spans="1:13" ht="27" customHeight="1">
       <c r="A19" s="5"/>
-      <c r="B19" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
+      <c r="B19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="6">
+        <v>3</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6">
+        <f>$C19*H$7</f>
+        <v>6</v>
+      </c>
+      <c r="I19" s="6">
+        <f>$C19*I$7</f>
+        <v>882</v>
+      </c>
+      <c r="J19" s="6">
+        <f>$C19*J$7</f>
+        <v>822</v>
+      </c>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
     </row>
     <row r="20" spans="1:13" ht="27" customHeight="1">
       <c r="A20" s="5"/>
-      <c r="B20" s="4" t="s">
-        <v>34</v>
+      <c r="B20" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="C20" s="6">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>28</v>
@@ -1343,19 +1391,21 @@
       <c r="E20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="6"/>
+      <c r="F20" s="6">
+        <v>9</v>
+      </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6">
-        <f>$C$20*H5</f>
-        <v>54</v>
+        <f>SUM(H17:H19)</f>
+        <v>8</v>
       </c>
       <c r="I20" s="6">
-        <f t="shared" ref="I20:J20" si="2">$C$20*I5</f>
-        <v>7938</v>
+        <f t="shared" ref="I20:J20" si="1">SUM(I17:I19)</f>
+        <v>1468</v>
       </c>
       <c r="J20" s="6">
-        <f t="shared" si="2"/>
-        <v>7398</v>
+        <f t="shared" si="1"/>
+        <v>1398</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
@@ -1363,20 +1413,20 @@
     </row>
     <row r="21" spans="1:13" ht="27" customHeight="1">
       <c r="A21" s="5"/>
-      <c r="B21" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
+      <c r="B21" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
     </row>
     <row r="22" spans="1:13" ht="27" customHeight="1">
       <c r="A22" s="5"/>
@@ -1384,7 +1434,7 @@
         <v>34</v>
       </c>
       <c r="C22" s="6">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>28</v>
@@ -1395,16 +1445,16 @@
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6">
-        <f>$C22*H5</f>
-        <v>128</v>
+        <f>$C$22*H7</f>
+        <v>54</v>
       </c>
       <c r="I22" s="6">
-        <f t="shared" ref="I22:J22" si="3">$C22*I5</f>
-        <v>18816</v>
+        <f t="shared" ref="I22:J22" si="2">$C$22*I7</f>
+        <v>7938</v>
       </c>
       <c r="J22" s="6">
-        <f t="shared" si="3"/>
-        <v>17536</v>
+        <f t="shared" si="2"/>
+        <v>7398</v>
       </c>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
@@ -1412,20 +1462,20 @@
     </row>
     <row r="23" spans="1:13" ht="27" customHeight="1">
       <c r="A23" s="5"/>
-      <c r="B23" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
+      <c r="B23" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
     </row>
     <row r="24" spans="1:13" ht="27" customHeight="1">
       <c r="A24" s="5"/>
@@ -1433,7 +1483,7 @@
         <v>34</v>
       </c>
       <c r="C24" s="6">
-        <v>216</v>
+        <v>16</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>28</v>
@@ -1441,48 +1491,50 @@
       <c r="E24" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="6"/>
+      <c r="F24" s="6">
+        <v>12</v>
+      </c>
       <c r="G24" s="6"/>
       <c r="H24" s="6">
-        <f>$C24*H5</f>
-        <v>432</v>
+        <f>$C24*H7</f>
+        <v>32</v>
       </c>
       <c r="I24" s="6">
-        <f t="shared" ref="I24:J24" si="4">$C24*I5</f>
-        <v>63504</v>
+        <f t="shared" ref="I24:J24" si="3">$C24*I7</f>
+        <v>4704</v>
       </c>
       <c r="J24" s="6">
-        <f t="shared" si="4"/>
-        <v>59184</v>
+        <f t="shared" si="3"/>
+        <v>4384</v>
       </c>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="1:13" s="2" customFormat="1" ht="27" customHeight="1">
-      <c r="A25" s="3"/>
-      <c r="B25" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
+    <row r="25" spans="1:13" ht="27" customHeight="1">
+      <c r="A25" s="5"/>
+      <c r="B25" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
     </row>
     <row r="26" spans="1:13" ht="27" customHeight="1">
       <c r="A26" s="5"/>
       <c r="B26" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C26" s="6">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>28</v>
@@ -1493,74 +1545,65 @@
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6">
-        <f>$C26*H18</f>
-        <v>24</v>
+        <f>$C26*H7</f>
+        <v>54</v>
       </c>
       <c r="I26" s="6">
-        <f>$C26*I18</f>
-        <v>4112</v>
+        <f t="shared" ref="I26:J26" si="4">$C26*I7</f>
+        <v>7938</v>
       </c>
       <c r="J26" s="6">
-        <f t="shared" ref="I26:J26" si="5">$C26*J18</f>
-        <v>3892</v>
+        <f t="shared" si="4"/>
+        <v>7398</v>
       </c>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
     </row>
-    <row r="27" spans="1:13" ht="27" customHeight="1">
-      <c r="A27" s="5"/>
-      <c r="B27" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="6">
-        <v>6</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6">
-        <f>$C27*H5</f>
-        <v>12</v>
-      </c>
-      <c r="I27" s="6">
-        <f>$C27*I5</f>
-        <v>1764</v>
-      </c>
-      <c r="J27" s="6">
-        <f t="shared" ref="I27:J27" si="6">$C27*J5</f>
-        <v>1644</v>
-      </c>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
+    <row r="27" spans="1:13" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A27" s="3"/>
+      <c r="B27" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
     </row>
     <row r="28" spans="1:13" ht="27" customHeight="1">
       <c r="A28" s="5"/>
-      <c r="B28" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
+      <c r="B28" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="6">
+        <v>2</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6">
-        <f>SUM(H26:H27)</f>
-        <v>36</v>
+        <f>$C28*H20</f>
+        <v>16</v>
       </c>
       <c r="I28" s="6">
-        <f>SUM(I26:I27)</f>
-        <v>5876</v>
+        <f>$C28*I20</f>
+        <v>2936</v>
       </c>
       <c r="J28" s="6">
-        <f>SUM(J26:J27)</f>
-        <v>5536</v>
+        <f t="shared" ref="J28" si="5">$C28*J20</f>
+        <v>2796</v>
       </c>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
@@ -1568,48 +1611,57 @@
     </row>
     <row r="29" spans="1:13" ht="27" customHeight="1">
       <c r="A29" s="5"/>
-      <c r="B29" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
+      <c r="B29" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="6">
+        <v>6</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6">
+        <f>$C29*H7</f>
+        <v>12</v>
+      </c>
+      <c r="I29" s="6">
+        <f>$C29*I7</f>
+        <v>1764</v>
+      </c>
+      <c r="J29" s="6">
+        <f t="shared" ref="J29" si="6">$C29*J7</f>
+        <v>1644</v>
+      </c>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
     </row>
     <row r="30" spans="1:13" ht="27" customHeight="1">
       <c r="A30" s="5"/>
-      <c r="B30" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="6">
-        <v>2</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="B30" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6">
-        <f>$C30*H22</f>
-        <v>256</v>
+        <f>SUM(H28:H29)</f>
+        <v>28</v>
       </c>
       <c r="I30" s="6">
-        <f>$C30*I22</f>
-        <v>37632</v>
+        <f>SUM(I28:I29)</f>
+        <v>4700</v>
       </c>
       <c r="J30" s="6">
-        <f t="shared" ref="I30:J30" si="7">$C30*J22</f>
-        <v>35072</v>
+        <f>SUM(J28:J29)</f>
+        <v>4440</v>
       </c>
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
@@ -1617,57 +1669,48 @@
     </row>
     <row r="31" spans="1:13" ht="27" customHeight="1">
       <c r="A31" s="5"/>
-      <c r="B31" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="6">
-        <v>3</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6">
-        <f>$C31*H28</f>
-        <v>108</v>
-      </c>
-      <c r="I31" s="6">
-        <f t="shared" ref="I31:J31" si="8">$C31*I28</f>
-        <v>17628</v>
-      </c>
-      <c r="J31" s="6">
-        <f t="shared" si="8"/>
-        <v>16608</v>
-      </c>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
+      <c r="B31" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
     </row>
     <row r="32" spans="1:13" ht="27" customHeight="1">
       <c r="A32" s="5"/>
-      <c r="B32" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
+      <c r="B32" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="6">
+        <v>2</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6">
-        <f>SUM(H30:H31)</f>
-        <v>364</v>
+        <f>$C32*H24</f>
+        <v>64</v>
       </c>
       <c r="I32" s="6">
-        <f t="shared" ref="I32:J32" si="9">SUM(I30:I31)</f>
-        <v>55260</v>
+        <f>$C32*I24</f>
+        <v>9408</v>
       </c>
       <c r="J32" s="6">
-        <f t="shared" si="9"/>
-        <v>51680</v>
+        <f t="shared" ref="J32" si="7">$C32*J24</f>
+        <v>8768</v>
       </c>
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
@@ -1675,48 +1718,57 @@
     </row>
     <row r="33" spans="1:13" ht="27" customHeight="1">
       <c r="A33" s="5"/>
-      <c r="B33" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
+      <c r="B33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="6">
+        <v>3</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6">
+        <f>$C33*H30</f>
+        <v>84</v>
+      </c>
+      <c r="I33" s="6">
+        <f t="shared" ref="I33:J33" si="8">$C33*I30</f>
+        <v>14100</v>
+      </c>
+      <c r="J33" s="6">
+        <f t="shared" si="8"/>
+        <v>13320</v>
+      </c>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
     </row>
     <row r="34" spans="1:13" ht="27" customHeight="1">
       <c r="A34" s="5"/>
-      <c r="B34" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="6">
-        <v>5</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="B34" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6">
-        <f>$C34*H22</f>
-        <v>640</v>
+        <f>SUM(H32:H33)</f>
+        <v>148</v>
       </c>
       <c r="I34" s="6">
-        <f t="shared" ref="I34:J34" si="10">$C34*I22</f>
-        <v>94080</v>
+        <f t="shared" ref="I34:J34" si="9">SUM(I32:I33)</f>
+        <v>23508</v>
       </c>
       <c r="J34" s="6">
-        <f t="shared" si="10"/>
-        <v>87680</v>
+        <f t="shared" si="9"/>
+        <v>22088</v>
       </c>
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
@@ -1724,57 +1776,48 @@
     </row>
     <row r="35" spans="1:13" ht="27" customHeight="1">
       <c r="A35" s="5"/>
-      <c r="B35" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="6">
-        <v>6</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6">
-        <f>$C35*H28</f>
-        <v>216</v>
-      </c>
-      <c r="I35" s="6">
-        <f t="shared" ref="I35:J35" si="11">$C35*I28</f>
-        <v>35256</v>
-      </c>
-      <c r="J35" s="6">
-        <f t="shared" si="11"/>
-        <v>33216</v>
-      </c>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
+      <c r="B35" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
     </row>
     <row r="36" spans="1:13" ht="27" customHeight="1">
       <c r="A36" s="5"/>
-      <c r="B36" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
+      <c r="B36" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="6">
+        <v>1</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6">
-        <f>SUM(H34:H35)</f>
-        <v>856</v>
+        <f>$C36*H24</f>
+        <v>32</v>
       </c>
       <c r="I36" s="6">
-        <f t="shared" ref="I36" si="12">SUM(I34:I35)</f>
-        <v>129336</v>
+        <f t="shared" ref="I36:J36" si="10">$C36*I24</f>
+        <v>4704</v>
       </c>
       <c r="J36" s="6">
-        <f t="shared" ref="J36" si="13">SUM(J34:J35)</f>
-        <v>120896</v>
+        <f t="shared" si="10"/>
+        <v>4384</v>
       </c>
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
@@ -1782,48 +1825,57 @@
     </row>
     <row r="37" spans="1:13" ht="27" customHeight="1">
       <c r="A37" s="5"/>
-      <c r="B37" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="9"/>
-      <c r="M37" s="9"/>
+      <c r="B37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="6">
+        <v>2</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6">
+        <f>$C37*H30</f>
+        <v>56</v>
+      </c>
+      <c r="I37" s="6">
+        <f t="shared" ref="I37:J37" si="11">$C37*I30</f>
+        <v>9400</v>
+      </c>
+      <c r="J37" s="6">
+        <f t="shared" si="11"/>
+        <v>8880</v>
+      </c>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
     </row>
     <row r="38" spans="1:13" ht="27" customHeight="1">
       <c r="A38" s="5"/>
-      <c r="B38" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" s="6">
-        <v>1</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="B38" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6">
-        <f>$C38*H24</f>
-        <v>432</v>
+        <f>SUM(H36:H37)</f>
+        <v>88</v>
       </c>
       <c r="I38" s="6">
-        <f t="shared" ref="I38:J38" si="14">$C38*I24</f>
-        <v>63504</v>
+        <f t="shared" ref="I38" si="12">SUM(I36:I37)</f>
+        <v>14104</v>
       </c>
       <c r="J38" s="6">
-        <f t="shared" si="14"/>
-        <v>59184</v>
+        <f t="shared" ref="J38" si="13">SUM(J36:J37)</f>
+        <v>13264</v>
       </c>
       <c r="K38" s="6"/>
       <c r="L38" s="6"/>
@@ -1831,210 +1883,336 @@
     </row>
     <row r="39" spans="1:13" ht="27" customHeight="1">
       <c r="A39" s="5"/>
-      <c r="B39" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C39" s="6">
-        <v>2</v>
-      </c>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
-      <c r="M39" s="6"/>
+      <c r="B39" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="15"/>
     </row>
     <row r="40" spans="1:13" ht="27" customHeight="1">
       <c r="A40" s="5"/>
-      <c r="B40" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
-      <c r="J40" s="9"/>
-      <c r="K40" s="9"/>
-      <c r="L40" s="9"/>
-      <c r="M40" s="9"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
     </row>
     <row r="41" spans="1:13" ht="27" customHeight="1">
       <c r="A41" s="5"/>
-      <c r="B41" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41" s="6">
-        <v>2</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
-      <c r="H41" s="6">
-        <f>$C41*H24</f>
-        <v>864</v>
-      </c>
-      <c r="I41" s="6">
-        <f t="shared" ref="I41:J41" si="15">$C41*I24</f>
-        <v>127008</v>
-      </c>
-      <c r="J41" s="6">
-        <f t="shared" si="15"/>
-        <v>118368</v>
-      </c>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
       <c r="K41" s="6"/>
       <c r="L41" s="6"/>
       <c r="M41" s="6"/>
     </row>
     <row r="42" spans="1:13" ht="27" customHeight="1">
       <c r="A42" s="5"/>
-      <c r="B42" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C42" s="6">
-        <v>1</v>
-      </c>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
-      <c r="L42" s="6"/>
-      <c r="M42" s="6"/>
+      <c r="B42" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
     </row>
     <row r="43" spans="1:13" ht="27" customHeight="1">
       <c r="A43" s="5"/>
       <c r="B43" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C43" s="6">
         <v>1</v>
       </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
+      <c r="D43" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
+      <c r="H43" s="6">
+        <f>$C43*H26</f>
+        <v>54</v>
+      </c>
+      <c r="I43" s="6">
+        <f t="shared" ref="I43:J43" si="14">$C43*I26</f>
+        <v>7938</v>
+      </c>
+      <c r="J43" s="6">
+        <f t="shared" si="14"/>
+        <v>7398</v>
+      </c>
       <c r="K43" s="6"/>
       <c r="L43" s="6"/>
       <c r="M43" s="6"/>
     </row>
     <row r="44" spans="1:13" ht="27" customHeight="1">
       <c r="A44" s="5"/>
-      <c r="B44" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
-      <c r="L44" s="9"/>
-      <c r="M44" s="9"/>
+      <c r="B44" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="6">
+        <v>2</v>
+      </c>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="6"/>
+      <c r="K44" s="6"/>
+      <c r="L44" s="6"/>
+      <c r="M44" s="6"/>
     </row>
     <row r="45" spans="1:13" ht="27" customHeight="1">
       <c r="A45" s="5"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
-      <c r="M45" s="6"/>
+      <c r="B45" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
     </row>
     <row r="46" spans="1:13" ht="27" customHeight="1">
       <c r="A46" s="5"/>
-      <c r="B46" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
+      <c r="B46" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" s="6">
+        <v>2</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6">
+        <f>$C46*H26</f>
+        <v>108</v>
+      </c>
+      <c r="I46" s="6">
+        <f t="shared" ref="I46:J46" si="15">$C46*I26</f>
+        <v>15876</v>
+      </c>
+      <c r="J46" s="6">
+        <f t="shared" si="15"/>
+        <v>14796</v>
+      </c>
+      <c r="K46" s="6"/>
+      <c r="L46" s="6"/>
+      <c r="M46" s="6"/>
     </row>
     <row r="47" spans="1:13" ht="27" customHeight="1">
       <c r="A47" s="5"/>
       <c r="B47" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C47" s="6"/>
+        <v>27</v>
+      </c>
+      <c r="C47" s="6">
+        <v>1</v>
+      </c>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="6">
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+    </row>
+    <row r="48" spans="1:13" ht="27" customHeight="1">
+      <c r="A48" s="5"/>
+      <c r="B48" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" s="6">
+        <v>1</v>
+      </c>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
+      <c r="K48" s="6"/>
+      <c r="L48" s="6"/>
+      <c r="M48" s="6"/>
+    </row>
+    <row r="49" spans="1:13" ht="27" customHeight="1">
+      <c r="A49" s="5"/>
+      <c r="B49" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11"/>
+    </row>
+    <row r="50" spans="1:13" ht="27" customHeight="1">
+      <c r="A50" s="5"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="6"/>
+      <c r="K50" s="6"/>
+      <c r="L50" s="6"/>
+      <c r="M50" s="6"/>
+    </row>
+    <row r="51" spans="1:13" ht="27" customHeight="1">
+      <c r="A51" s="5"/>
+      <c r="B51" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="11"/>
+      <c r="M51" s="11"/>
+    </row>
+    <row r="52" spans="1:13" ht="27" customHeight="1">
+      <c r="A52" s="5"/>
+      <c r="B52" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6">
         <v>112</v>
       </c>
-      <c r="I47" s="6">
+      <c r="I52" s="6">
         <v>41509</v>
       </c>
-      <c r="J47" s="6">
+      <c r="J52" s="6">
         <v>166036</v>
       </c>
-      <c r="K47" s="6">
+      <c r="K52" s="6">
         <v>336</v>
       </c>
-      <c r="L47" s="6">
+      <c r="L52" s="6">
         <v>224</v>
       </c>
-      <c r="M47" s="6">
+      <c r="M52" s="6">
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="6:7" ht="27" customHeight="1">
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-    </row>
-    <row r="54" spans="6:7" ht="27" customHeight="1">
-      <c r="F54" s="7"/>
-      <c r="G54" s="7"/>
+    <row r="58" spans="1:13" ht="27" customHeight="1">
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+    </row>
+    <row r="59" spans="1:13" ht="27" customHeight="1">
+      <c r="B59" s="12">
+        <v>267000000</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+    </row>
+    <row r="60" spans="1:13" ht="27" customHeight="1">
+      <c r="B60" s="12">
+        <f>1/B59</f>
+        <v>3.7453183520599249E-9</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="27" customHeight="1">
+      <c r="B61" s="12">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="27" customHeight="1">
+      <c r="B62" s="12">
+        <f>B61/B60</f>
+        <v>10680.000000000002</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
     <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B27:M27"/>
+    <mergeCell ref="B31:M31"/>
+    <mergeCell ref="B35:M35"/>
+    <mergeCell ref="B51:M51"/>
+    <mergeCell ref="B42:M42"/>
+    <mergeCell ref="B45:M45"/>
+    <mergeCell ref="B16:M16"/>
+    <mergeCell ref="B23:M23"/>
     <mergeCell ref="B25:M25"/>
-    <mergeCell ref="B29:M29"/>
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B46:M46"/>
-    <mergeCell ref="B37:M37"/>
-    <mergeCell ref="B40:M40"/>
-    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="B49:M49"/>
     <mergeCell ref="B21:M21"/>
-    <mergeCell ref="B23:M23"/>
-    <mergeCell ref="B44:M44"/>
-    <mergeCell ref="B19:M19"/>
+    <mergeCell ref="B39:M39"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added an appendix which includes our bill of materials. Added damped least squares writeup. Added functional units writeup. Converted Jacobian Pipeline to .eps.
</commit_message>
<xml_diff>
--- a/doc/design/bill_of_materials.xlsx
+++ b/doc/design/bill_of_materials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -492,9 +492,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -502,6 +499,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -993,8 +993,8 @@
   <dimension ref="A1:O91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B80" sqref="B80:O80"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0"/>
@@ -1061,22 +1061,22 @@
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A3" s="3"/>
@@ -1102,14 +1102,14 @@
         <v>0</v>
       </c>
       <c r="I3" s="13">
-        <f>H3/H$81</f>
+        <f t="shared" ref="I3:I14" si="0">H3/H$81</f>
         <v>0</v>
       </c>
       <c r="J3" s="6">
         <v>11</v>
       </c>
       <c r="K3" s="13">
-        <f>J3/J$81</f>
+        <f t="shared" ref="K3:K14" si="1">J3/J$81</f>
         <v>2.6500277048350959E-4</v>
       </c>
       <c r="L3" s="6">
@@ -1149,14 +1149,14 @@
         <v>0</v>
       </c>
       <c r="I4" s="13">
-        <f>H4/H$81</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4" s="6">
         <v>146</v>
       </c>
       <c r="K4" s="13">
-        <f>J4/J$81</f>
+        <f t="shared" si="1"/>
         <v>3.5173094991447639E-3</v>
       </c>
       <c r="L4" s="6">
@@ -1196,14 +1196,14 @@
         <v>2</v>
       </c>
       <c r="I5" s="13">
-        <f>H5/H$81</f>
+        <f t="shared" si="0"/>
         <v>1.7857142857142856E-2</v>
       </c>
       <c r="J5" s="6">
         <v>294</v>
       </c>
       <c r="K5" s="13">
-        <f>J5/J$81</f>
+        <f t="shared" si="1"/>
         <v>7.0828013201956206E-3</v>
       </c>
       <c r="L5" s="6">
@@ -1243,14 +1243,14 @@
         <v>0</v>
       </c>
       <c r="I6" s="13">
-        <f>H6/H$81</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J6" s="6">
         <v>642</v>
       </c>
       <c r="K6" s="13">
-        <f>J6/J$81</f>
+        <f t="shared" si="1"/>
         <v>1.5466525331855743E-2</v>
       </c>
       <c r="L6" s="6">
@@ -1290,14 +1290,14 @@
         <v>0</v>
       </c>
       <c r="I7" s="13">
-        <f>H7/H$81</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J7" s="6">
         <v>94</v>
       </c>
       <c r="K7" s="13">
-        <f>J7/J$81</f>
+        <f t="shared" si="1"/>
         <v>2.2645691295863548E-3</v>
       </c>
       <c r="L7" s="6">
@@ -1337,14 +1337,14 @@
         <v>7</v>
       </c>
       <c r="I8" s="13">
-        <f>H8/H$81</f>
+        <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
       <c r="J8" s="6">
         <v>2697</v>
       </c>
       <c r="K8" s="13">
-        <f>J8/J$81</f>
+        <f t="shared" si="1"/>
         <v>6.4973861090365945E-2</v>
       </c>
       <c r="L8" s="6">
@@ -1384,14 +1384,14 @@
         <v>7</v>
       </c>
       <c r="I9" s="13">
-        <f>H9/H$81</f>
+        <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
       <c r="J9" s="6">
         <v>2631</v>
       </c>
       <c r="K9" s="13">
-        <f>J9/J$81</f>
+        <f t="shared" si="1"/>
         <v>6.3383844467464881E-2</v>
       </c>
       <c r="L9" s="6">
@@ -1431,14 +1431,14 @@
         <v>1</v>
       </c>
       <c r="I10" s="13">
-        <f>H10/H$81</f>
+        <f t="shared" si="0"/>
         <v>8.9285714285714281E-3</v>
       </c>
       <c r="J10" s="6">
         <v>217</v>
       </c>
       <c r="K10" s="13">
-        <f>J10/J$81</f>
+        <f t="shared" si="1"/>
         <v>5.2277819268110532E-3</v>
       </c>
       <c r="L10" s="6">
@@ -1478,14 +1478,14 @@
         <v>1</v>
       </c>
       <c r="I11" s="13">
-        <f>H11/H$81</f>
+        <f t="shared" si="0"/>
         <v>8.9285714285714281E-3</v>
       </c>
       <c r="J11" s="6">
         <v>154</v>
       </c>
       <c r="K11" s="13">
-        <f>J11/J$81</f>
+        <f t="shared" si="1"/>
         <v>3.7100387867691344E-3</v>
       </c>
       <c r="L11" s="6">
@@ -1525,14 +1525,14 @@
         <v>0</v>
       </c>
       <c r="I12" s="13">
-        <f>H12/H$81</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J12" s="6">
         <v>55</v>
       </c>
       <c r="K12" s="13">
-        <f>J12/J$81</f>
+        <f t="shared" si="1"/>
         <v>1.3250138524175481E-3</v>
       </c>
       <c r="L12" s="6">
@@ -1572,14 +1572,14 @@
         <v>32</v>
       </c>
       <c r="I13" s="13">
-        <f>H13/H$81</f>
+        <f t="shared" si="0"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="J13" s="6">
         <v>3698</v>
       </c>
       <c r="K13" s="13">
-        <f>J13/J$81</f>
+        <f t="shared" si="1"/>
         <v>8.9089113204365314E-2</v>
       </c>
       <c r="L13" s="6">
@@ -1619,14 +1619,14 @@
         <v>574</v>
       </c>
       <c r="I14" s="13">
-        <f>H14/H$81</f>
+        <f t="shared" si="0"/>
         <v>5.125</v>
       </c>
       <c r="J14" s="6">
         <v>62872</v>
       </c>
       <c r="K14" s="13">
-        <f>J14/J$81</f>
+        <f t="shared" si="1"/>
         <v>1.5146594714399286</v>
       </c>
       <c r="L14" s="6">
@@ -1644,22 +1644,22 @@
     </row>
     <row r="15" spans="1:15" ht="27" customHeight="1">
       <c r="A15" s="5"/>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
     </row>
     <row r="16" spans="1:15" ht="27" customHeight="1">
       <c r="A16" s="5"/>
@@ -1698,15 +1698,15 @@
         <v>302</v>
       </c>
       <c r="M16" s="6">
-        <f t="shared" ref="M16:O16" si="0">$C16*M$4</f>
+        <f t="shared" ref="M16:O16" si="2">$C16*M$4</f>
         <v>0</v>
       </c>
       <c r="N16" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O16" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1716,7 +1716,7 @@
         <v>30</v>
       </c>
       <c r="C17" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>24</v>
@@ -1728,34 +1728,34 @@
       <c r="G17" s="6"/>
       <c r="H17" s="6">
         <f>$C17*H$5</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I17" s="13">
         <f>H17/H$81</f>
-        <v>1.7857142857142856E-2</v>
+        <v>3.5714285714285712E-2</v>
       </c>
       <c r="J17" s="6">
-        <f t="shared" ref="J17:O18" si="1">$C17*J$5</f>
-        <v>294</v>
+        <f t="shared" ref="J17:O18" si="3">$C17*J$5</f>
+        <v>588</v>
       </c>
       <c r="K17" s="13">
         <f>J17/J$81</f>
-        <v>7.0828013201956206E-3</v>
+        <v>1.4165602640391241E-2</v>
       </c>
       <c r="L17" s="6">
-        <f t="shared" si="1"/>
-        <v>274</v>
+        <f t="shared" si="3"/>
+        <v>548</v>
       </c>
       <c r="M17" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N17" s="6">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="O17" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1765,7 +1765,7 @@
         <v>29</v>
       </c>
       <c r="C18" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>24</v>
@@ -1777,34 +1777,34 @@
       <c r="G18" s="6"/>
       <c r="H18" s="6">
         <f>$C18*H$5</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I18" s="13">
         <f>H18/H$81</f>
-        <v>5.3571428571428568E-2</v>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="J18" s="6">
         <f>$C18*J$5</f>
-        <v>882</v>
+        <v>1176</v>
       </c>
       <c r="K18" s="13">
         <f>J18/J$81</f>
-        <v>2.1248403960586859E-2</v>
+        <v>2.8331205280782482E-2</v>
       </c>
       <c r="L18" s="6">
         <f>$C18*L$5</f>
-        <v>822</v>
+        <v>1096</v>
       </c>
       <c r="M18" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N18" s="6">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="O18" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1823,60 +1823,60 @@
         <v>25</v>
       </c>
       <c r="F19" s="6">
-        <f>2*F4+1*F5+F3</f>
-        <v>11</v>
+        <f>2*F4+2*F5+F3</f>
+        <v>14</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6">
         <f>SUM(H16:H18)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I19" s="13">
         <f>H19/H$81</f>
-        <v>7.1428571428571425E-2</v>
+        <v>0.10714285714285714</v>
       </c>
       <c r="J19" s="6">
-        <f t="shared" ref="J19:O19" si="2">SUM(J16:J18)</f>
-        <v>1468</v>
+        <f t="shared" ref="J19:O19" si="4">SUM(J16:J18)</f>
+        <v>2056</v>
       </c>
       <c r="K19" s="13">
         <f>J19/J$81</f>
-        <v>3.5365824279072006E-2</v>
+        <v>4.9531426919463252E-2</v>
       </c>
       <c r="L19" s="6">
-        <f t="shared" si="2"/>
-        <v>1398</v>
+        <f t="shared" si="4"/>
+        <v>1946</v>
       </c>
       <c r="M19" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N19" s="6">
-        <f t="shared" si="2"/>
-        <v>8</v>
+        <f t="shared" si="4"/>
+        <v>12</v>
       </c>
       <c r="O19" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="27" hidden="1" customHeight="1">
       <c r="A20" s="5"/>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="19"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="18"/>
       <c r="O20" s="10"/>
     </row>
     <row r="21" spans="1:15" ht="27" hidden="1" customHeight="1">
@@ -1904,7 +1904,7 @@
         <v>0.32142857142857145</v>
       </c>
       <c r="J21" s="6">
-        <f t="shared" ref="J21:O21" si="3">$C21*J5</f>
+        <f t="shared" ref="J21:O21" si="5">$C21*J5</f>
         <v>5292</v>
       </c>
       <c r="K21" s="13">
@@ -1912,19 +1912,19 @@
         <v>0.12749042376352115</v>
       </c>
       <c r="L21" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4932</v>
       </c>
       <c r="M21" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N21" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
       <c r="O21" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1953,7 +1953,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="6">
-        <f t="shared" ref="J22:O22" si="4">$C22*J3</f>
+        <f t="shared" ref="J22:O22" si="6">$C22*J3</f>
         <v>99</v>
       </c>
       <c r="K22" s="13">
@@ -1961,19 +1961,19 @@
         <v>2.3850249343515865E-3</v>
       </c>
       <c r="L22" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M22" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N22" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O22" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -2004,7 +2004,7 @@
         <v>0.32142857142857145</v>
       </c>
       <c r="J23" s="6">
-        <f t="shared" ref="J23:L23" si="5">SUM(J21:J22)</f>
+        <f t="shared" ref="J23:L23" si="7">SUM(J21:J22)</f>
         <v>5391</v>
       </c>
       <c r="K23" s="13">
@@ -2012,40 +2012,40 @@
         <v>0.12987544869787276</v>
       </c>
       <c r="L23" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4932</v>
       </c>
       <c r="M23" s="6">
-        <f t="shared" ref="M23" si="6">SUM(M21:M22)</f>
+        <f t="shared" ref="M23" si="8">SUM(M21:M22)</f>
         <v>0</v>
       </c>
       <c r="N23" s="6">
-        <f t="shared" ref="N23" si="7">SUM(N21:N22)</f>
+        <f t="shared" ref="N23" si="9">SUM(N21:N22)</f>
         <v>36</v>
       </c>
       <c r="O23" s="6">
-        <f t="shared" ref="O23" si="8">SUM(O21:O22)</f>
+        <f t="shared" ref="O23" si="10">SUM(O21:O22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="27" customHeight="1">
       <c r="A24" s="5"/>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
-      <c r="O24" s="16"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
     </row>
     <row r="25" spans="1:15" ht="27" customHeight="1">
       <c r="A25" s="5"/>
@@ -2072,7 +2072,7 @@
         <v>0.2857142857142857</v>
       </c>
       <c r="J25" s="6">
-        <f t="shared" ref="J25:O25" si="9">$C25*J5</f>
+        <f t="shared" ref="J25:O25" si="11">$C25*J5</f>
         <v>4704</v>
       </c>
       <c r="K25" s="13">
@@ -2080,19 +2080,19 @@
         <v>0.11332482112312993</v>
       </c>
       <c r="L25" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>4384</v>
       </c>
       <c r="M25" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N25" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>32</v>
       </c>
       <c r="O25" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -2121,7 +2121,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="6">
-        <f t="shared" ref="J26:O26" si="10">$C26*J3</f>
+        <f t="shared" ref="J26:O26" si="12">$C26*J3</f>
         <v>176</v>
       </c>
       <c r="K26" s="13">
@@ -2129,19 +2129,19 @@
         <v>4.2400443277361534E-3</v>
       </c>
       <c r="L26" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M26" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N26" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O26" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -2173,7 +2173,7 @@
         <v>0.2857142857142857</v>
       </c>
       <c r="J27" s="6">
-        <f t="shared" ref="J27:O27" si="11">SUM(J25:J26)</f>
+        <f t="shared" ref="J27:O27" si="13">SUM(J25:J26)</f>
         <v>4880</v>
       </c>
       <c r="K27" s="13">
@@ -2181,40 +2181,40 @@
         <v>0.11756486545086607</v>
       </c>
       <c r="L27" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>4384</v>
       </c>
       <c r="M27" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="N27" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>32</v>
       </c>
       <c r="O27" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="27" customHeight="1">
       <c r="A28" s="5"/>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="16"/>
-      <c r="O28" s="16"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
     </row>
     <row r="29" spans="1:15" ht="27" customHeight="1">
       <c r="A29" s="5"/>
@@ -2241,7 +2241,7 @@
         <v>0.10714285714285714</v>
       </c>
       <c r="J29" s="6">
-        <f t="shared" ref="J29:O29" si="12">$C29*J5</f>
+        <f t="shared" ref="J29:O29" si="14">$C29*J5</f>
         <v>1764</v>
       </c>
       <c r="K29" s="13">
@@ -2249,19 +2249,19 @@
         <v>4.2496807921173718E-2</v>
       </c>
       <c r="L29" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1644</v>
       </c>
       <c r="M29" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N29" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>12</v>
       </c>
       <c r="O29" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -2290,7 +2290,7 @@
         <v>0</v>
       </c>
       <c r="J30" s="6">
-        <f t="shared" ref="J30:O30" si="13">$C30*J3</f>
+        <f t="shared" ref="J30:O30" si="15">$C30*J3</f>
         <v>33</v>
       </c>
       <c r="K30" s="13">
@@ -2298,19 +2298,19 @@
         <v>7.9500831145052882E-4</v>
       </c>
       <c r="L30" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="M30" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N30" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="O30" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -2342,7 +2342,7 @@
         <v>0.10714285714285714</v>
       </c>
       <c r="J31" s="6">
-        <f t="shared" ref="J31:O31" si="14">SUM(J29:J30)</f>
+        <f t="shared" ref="J31:O31" si="16">SUM(J29:J30)</f>
         <v>1797</v>
       </c>
       <c r="K31" s="13">
@@ -2350,40 +2350,40 @@
         <v>4.329181623262425E-2</v>
       </c>
       <c r="L31" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1644</v>
       </c>
       <c r="M31" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="N31" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>12</v>
       </c>
       <c r="O31" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="27" customHeight="1">
       <c r="A32" s="5"/>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="16"/>
-      <c r="K32" s="16"/>
-      <c r="L32" s="16"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="16"/>
-      <c r="O32" s="16"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
     </row>
     <row r="33" spans="1:15" ht="27" customHeight="1">
       <c r="A33" s="5"/>
@@ -2408,7 +2408,7 @@
         <v>0.10714285714285714</v>
       </c>
       <c r="J33" s="6">
-        <f t="shared" ref="J33:O33" si="15">$C33*J5</f>
+        <f t="shared" ref="J33:O33" si="17">$C33*J5</f>
         <v>1764</v>
       </c>
       <c r="K33" s="13">
@@ -2416,19 +2416,19 @@
         <v>4.2496807921173718E-2</v>
       </c>
       <c r="L33" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1644</v>
       </c>
       <c r="M33" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="N33" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>12</v>
       </c>
       <c r="O33" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -2455,7 +2455,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="6">
-        <f t="shared" ref="J34:N34" si="16">$C34*J3</f>
+        <f t="shared" ref="J34:N34" si="18">$C34*J3</f>
         <v>66</v>
       </c>
       <c r="K34" s="13">
@@ -2463,15 +2463,15 @@
         <v>1.5900166229010576E-3</v>
       </c>
       <c r="L34" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="M34" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="N34" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="O34" s="6">
@@ -2505,7 +2505,7 @@
         <v>0.10714285714285714</v>
       </c>
       <c r="J35" s="6">
-        <f t="shared" ref="J35:O35" si="17">SUM(J33:J34)</f>
+        <f t="shared" ref="J35:O35" si="19">SUM(J33:J34)</f>
         <v>1830</v>
       </c>
       <c r="K35" s="13">
@@ -2513,40 +2513,40 @@
         <v>4.4086824544074782E-2</v>
       </c>
       <c r="L35" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1644</v>
       </c>
       <c r="M35" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="N35" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>12</v>
       </c>
       <c r="O35" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="27" customHeight="1">
       <c r="A36" s="5"/>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="16"/>
-      <c r="K36" s="16"/>
-      <c r="L36" s="16"/>
-      <c r="M36" s="16"/>
-      <c r="N36" s="16"/>
-      <c r="O36" s="16"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
     </row>
     <row r="37" spans="1:15" ht="27" customHeight="1">
       <c r="A37" s="5"/>
@@ -2573,7 +2573,7 @@
         <v>0.6428571428571429</v>
       </c>
       <c r="J37" s="6">
-        <f t="shared" ref="J37:O37" si="18">$C37*J5</f>
+        <f t="shared" ref="J37:O37" si="20">$C37*J5</f>
         <v>10584</v>
       </c>
       <c r="K37" s="13">
@@ -2581,19 +2581,19 @@
         <v>0.25498084752704231</v>
       </c>
       <c r="L37" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>9864</v>
       </c>
       <c r="M37" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N37" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>72</v>
       </c>
       <c r="O37" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -2622,7 +2622,7 @@
         <v>0</v>
       </c>
       <c r="J38" s="6">
-        <f t="shared" ref="J38:O38" si="19">$C38*J3</f>
+        <f t="shared" ref="J38:O38" si="21">$C38*J3</f>
         <v>396</v>
       </c>
       <c r="K38" s="13">
@@ -2630,19 +2630,19 @@
         <v>9.5400997374063459E-3</v>
       </c>
       <c r="L38" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="M38" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="N38" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="O38" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -2674,7 +2674,7 @@
         <v>0.6428571428571429</v>
       </c>
       <c r="J39" s="6">
-        <f t="shared" ref="J39:O39" si="20">SUM(J37:J38)</f>
+        <f t="shared" ref="J39:O39" si="22">SUM(J37:J38)</f>
         <v>10980</v>
       </c>
       <c r="K39" s="13">
@@ -2682,40 +2682,40 @@
         <v>0.26452094726444869</v>
       </c>
       <c r="L39" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>9864</v>
       </c>
       <c r="M39" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="N39" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>72</v>
       </c>
       <c r="O39" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="27" customHeight="1">
       <c r="A40" s="5"/>
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
-      <c r="I40" s="16"/>
-      <c r="J40" s="16"/>
-      <c r="K40" s="16"/>
-      <c r="L40" s="16"/>
-      <c r="M40" s="16"/>
-      <c r="N40" s="16"/>
-      <c r="O40" s="16"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
     </row>
     <row r="41" spans="1:15" ht="27" customHeight="1">
       <c r="A41" s="5"/>
@@ -2740,7 +2740,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="6">
-        <f t="shared" ref="J41:N41" si="21">$C41*J7</f>
+        <f t="shared" ref="J41:N41" si="23">$C41*J7</f>
         <v>94</v>
       </c>
       <c r="K41" s="13">
@@ -2748,15 +2748,15 @@
         <v>2.2645691295863548E-3</v>
       </c>
       <c r="L41" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="M41" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="N41" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="O41" s="10"/>
@@ -2784,7 +2784,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="6">
-        <f t="shared" ref="J42:N42" si="22">$C42*J6</f>
+        <f t="shared" ref="J42:N42" si="24">$C42*J6</f>
         <v>3210</v>
       </c>
       <c r="K42" s="13">
@@ -2792,15 +2792,15 @@
         <v>7.7332626659278716E-2</v>
       </c>
       <c r="L42" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M42" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="N42" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="O42" s="10"/>
@@ -2828,7 +2828,7 @@
         <v>0.44642857142857145</v>
       </c>
       <c r="J43" s="6">
-        <f t="shared" ref="J43:N43" si="23">$C43*J5</f>
+        <f t="shared" ref="J43:N43" si="25">$C43*J5</f>
         <v>7350</v>
       </c>
       <c r="K43" s="13">
@@ -2836,15 +2836,15 @@
         <v>0.17707003300489049</v>
       </c>
       <c r="L43" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>6850</v>
       </c>
       <c r="M43" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N43" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>50</v>
       </c>
       <c r="O43" s="10"/>
@@ -2872,7 +2872,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="6">
-        <f t="shared" ref="J44:N44" si="24">$C44*J3</f>
+        <f t="shared" ref="J44:N44" si="26">$C44*J3</f>
         <v>275</v>
       </c>
       <c r="K44" s="13">
@@ -2880,15 +2880,15 @@
         <v>6.6250692620877403E-3</v>
       </c>
       <c r="L44" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="M44" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="N44" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O44" s="10"/>
@@ -2942,21 +2942,21 @@
     </row>
     <row r="46" spans="1:15" ht="27" customHeight="1">
       <c r="A46" s="5"/>
-      <c r="B46" s="17" t="s">
+      <c r="B46" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
-      <c r="N46" s="19"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="17"/>
+      <c r="L46" s="17"/>
+      <c r="M46" s="17"/>
+      <c r="N46" s="18"/>
       <c r="O46" s="15"/>
     </row>
     <row r="47" spans="1:15" ht="27" customHeight="1">
@@ -3128,22 +3128,22 @@
     </row>
     <row r="51" spans="1:15" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A51" s="3"/>
-      <c r="B51" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="16"/>
-      <c r="H51" s="16"/>
-      <c r="I51" s="16"/>
-      <c r="J51" s="16"/>
-      <c r="K51" s="16"/>
-      <c r="L51" s="16"/>
-      <c r="M51" s="16"/>
-      <c r="N51" s="16"/>
-      <c r="O51" s="16"/>
+      <c r="B51" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="19"/>
+      <c r="K51" s="19"/>
+      <c r="L51" s="19"/>
+      <c r="M51" s="19"/>
+      <c r="N51" s="19"/>
+      <c r="O51" s="19"/>
     </row>
     <row r="52" spans="1:15" ht="27" customHeight="1">
       <c r="A52" s="5"/>
@@ -3163,23 +3163,23 @@
       <c r="G52" s="6"/>
       <c r="H52" s="6">
         <f>$C52*H19</f>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="I52" s="13">
         <f>H52/H$81</f>
-        <v>0.14285714285714285</v>
+        <v>0.21428571428571427</v>
       </c>
       <c r="J52" s="6">
         <f>$C52*J19</f>
-        <v>2936</v>
+        <v>4112</v>
       </c>
       <c r="K52" s="13">
         <f>J52/J$81</f>
-        <v>7.0731648558144011E-2</v>
+        <v>9.9062853838926504E-2</v>
       </c>
       <c r="L52" s="6">
         <f>$C52*L19</f>
-        <v>2796</v>
+        <v>3892</v>
       </c>
       <c r="M52" s="6">
         <f>$C52*M19</f>
@@ -3187,7 +3187,7 @@
       </c>
       <c r="N52" s="6">
         <f>$C52*N19</f>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="O52" s="6">
         <f>$C52*O19</f>
@@ -3253,59 +3253,59 @@
       <c r="E54" s="6"/>
       <c r="F54" s="6">
         <f>1*F19+1*F5</f>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G54" s="6"/>
       <c r="H54" s="6">
         <f>SUM(H52:H53)</f>
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="I54" s="13">
         <f>H54/H$81</f>
-        <v>0.25</v>
+        <v>0.32142857142857145</v>
       </c>
       <c r="J54" s="6">
-        <f t="shared" ref="J54:O54" si="25">SUM(J52:J53)</f>
-        <v>4700</v>
+        <f t="shared" ref="J54:O54" si="27">SUM(J52:J53)</f>
+        <v>5876</v>
       </c>
       <c r="K54" s="13">
         <f>J54/J$81</f>
-        <v>0.11322845647931774</v>
+        <v>0.14155966176010021</v>
       </c>
       <c r="L54" s="6">
-        <f t="shared" si="25"/>
-        <v>4440</v>
+        <f t="shared" si="27"/>
+        <v>5536</v>
       </c>
       <c r="M54" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="N54" s="6">
-        <f t="shared" si="25"/>
-        <v>28</v>
+        <f t="shared" si="27"/>
+        <v>36</v>
       </c>
       <c r="O54" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:15" ht="27" hidden="1" customHeight="1">
       <c r="A55" s="5"/>
-      <c r="B55" s="17" t="s">
+      <c r="B55" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="18"/>
-      <c r="I55" s="18"/>
-      <c r="J55" s="18"/>
-      <c r="K55" s="18"/>
-      <c r="L55" s="18"/>
-      <c r="M55" s="18"/>
-      <c r="N55" s="19"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="17"/>
+      <c r="J55" s="17"/>
+      <c r="K55" s="17"/>
+      <c r="L55" s="17"/>
+      <c r="M55" s="17"/>
+      <c r="N55" s="18"/>
       <c r="O55" s="10"/>
     </row>
     <row r="56" spans="1:15" ht="27" hidden="1" customHeight="1">
@@ -3375,31 +3375,31 @@
       <c r="G57" s="6"/>
       <c r="H57" s="6">
         <f>$C57*H54</f>
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="I57" s="13">
         <f>H57/H$81</f>
-        <v>0.75</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="J57" s="6">
-        <f t="shared" ref="J57:N57" si="26">$C57*J54</f>
-        <v>14100</v>
+        <f t="shared" ref="J57:N57" si="28">$C57*J54</f>
+        <v>17628</v>
       </c>
       <c r="K57" s="13">
         <f>J57/J$81</f>
-        <v>0.33968536943795319</v>
+        <v>0.42467898528030068</v>
       </c>
       <c r="L57" s="6">
-        <f t="shared" si="26"/>
-        <v>13320</v>
+        <f t="shared" si="28"/>
+        <v>16608</v>
       </c>
       <c r="M57" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="N57" s="6">
-        <f t="shared" si="26"/>
-        <v>84</v>
+        <f t="shared" si="28"/>
+        <v>108</v>
       </c>
       <c r="O57" s="6">
         <f>$C57*O54</f>
@@ -3418,55 +3418,55 @@
       <c r="G58" s="6"/>
       <c r="H58" s="6">
         <f>SUM(H56:H57)</f>
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="I58" s="13">
         <f>H58/H$81</f>
-        <v>1.3214285714285714</v>
+        <v>1.5357142857142858</v>
       </c>
       <c r="J58" s="6">
-        <f t="shared" ref="J58:O58" si="27">SUM(J56:J57)</f>
-        <v>23860</v>
+        <f t="shared" ref="J58:O58" si="29">SUM(J56:J57)</f>
+        <v>27388</v>
       </c>
       <c r="K58" s="13">
         <f>J58/J$81</f>
-        <v>0.57481510033968541</v>
+        <v>0.65980871618203285</v>
       </c>
       <c r="L58" s="6">
-        <f t="shared" si="27"/>
-        <v>22088</v>
+        <f t="shared" si="29"/>
+        <v>25376</v>
       </c>
       <c r="M58" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="N58" s="6">
-        <f t="shared" si="27"/>
-        <v>148</v>
+        <f t="shared" si="29"/>
+        <v>172</v>
       </c>
       <c r="O58" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:15" ht="27" customHeight="1">
       <c r="A59" s="5"/>
-      <c r="B59" s="16" t="s">
+      <c r="B59" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C59" s="16"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="16"/>
-      <c r="F59" s="16"/>
-      <c r="G59" s="16"/>
-      <c r="H59" s="16"/>
-      <c r="I59" s="16"/>
-      <c r="J59" s="16"/>
-      <c r="K59" s="16"/>
-      <c r="L59" s="16"/>
-      <c r="M59" s="16"/>
-      <c r="N59" s="16"/>
-      <c r="O59" s="16"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="19"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="19"/>
+      <c r="J59" s="19"/>
+      <c r="K59" s="19"/>
+      <c r="L59" s="19"/>
+      <c r="M59" s="19"/>
+      <c r="N59" s="19"/>
+      <c r="O59" s="19"/>
     </row>
     <row r="60" spans="1:15" ht="27" customHeight="1">
       <c r="A60" s="5"/>
@@ -3486,34 +3486,34 @@
       <c r="G60" s="6"/>
       <c r="H60" s="6">
         <f>$C60*H52</f>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="I60" s="13">
         <f>H60/H$81</f>
-        <v>0.14285714285714285</v>
+        <v>0.21428571428571427</v>
       </c>
       <c r="J60" s="6">
         <f>$C60*J54</f>
-        <v>4700</v>
+        <v>5876</v>
       </c>
       <c r="K60" s="13">
         <f>J60/J$81</f>
-        <v>0.11322845647931774</v>
+        <v>0.14155966176010021</v>
       </c>
       <c r="L60" s="6">
-        <f t="shared" ref="L60:O60" si="28">$C60*L54</f>
-        <v>4440</v>
+        <f t="shared" ref="L60:O60" si="30">$C60*L54</f>
+        <v>5536</v>
       </c>
       <c r="M60" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="N60" s="6">
-        <f t="shared" si="28"/>
-        <v>28</v>
+        <f t="shared" si="30"/>
+        <v>36</v>
       </c>
       <c r="O60" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
@@ -3576,7 +3576,7 @@
       <c r="E62" s="6"/>
       <c r="F62" s="6">
         <f>6*F54+1*F27</f>
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="G62" s="6"/>
       <c r="H62" s="6">
@@ -3589,47 +3589,47 @@
       </c>
       <c r="J62" s="6">
         <f>SUM(J60:J61)</f>
-        <v>9580</v>
+        <v>10756</v>
       </c>
       <c r="K62" s="13">
         <f>J62/J$81</f>
-        <v>0.23079332193018381</v>
+        <v>0.25912452721096629</v>
       </c>
       <c r="L62" s="6">
-        <f t="shared" ref="L62:O62" si="29">SUM(L60:L61)</f>
-        <v>8824</v>
+        <f t="shared" ref="L62:O62" si="31">SUM(L60:L61)</f>
+        <v>9920</v>
       </c>
       <c r="M62" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="N62" s="6">
-        <f t="shared" si="29"/>
-        <v>60</v>
+        <f t="shared" si="31"/>
+        <v>68</v>
       </c>
       <c r="O62" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:15" ht="27" customHeight="1">
       <c r="A63" s="5"/>
-      <c r="B63" s="16" t="s">
+      <c r="B63" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C63" s="16"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
-      <c r="H63" s="16"/>
-      <c r="I63" s="16"/>
-      <c r="J63" s="16"/>
-      <c r="K63" s="16"/>
-      <c r="L63" s="16"/>
-      <c r="M63" s="16"/>
-      <c r="N63" s="16"/>
-      <c r="O63" s="16"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
+      <c r="J63" s="19"/>
+      <c r="K63" s="19"/>
+      <c r="L63" s="19"/>
+      <c r="M63" s="19"/>
+      <c r="N63" s="19"/>
+      <c r="O63" s="19"/>
     </row>
     <row r="64" spans="1:15" ht="27" customHeight="1">
       <c r="A64" s="5"/>
@@ -3757,7 +3757,7 @@
         <v>0.10714285714285714</v>
       </c>
       <c r="J66" s="6">
-        <f t="shared" ref="J66:O66" si="30">SUM(J64:J65)</f>
+        <f t="shared" ref="J66:O66" si="32">SUM(J64:J65)</f>
         <v>1830</v>
       </c>
       <c r="K66" s="13">
@@ -3765,39 +3765,39 @@
         <v>4.4086824544074782E-2</v>
       </c>
       <c r="L66" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>1644</v>
       </c>
       <c r="M66" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="N66" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>12</v>
       </c>
       <c r="O66" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:15" ht="27" hidden="1" customHeight="1">
       <c r="A67" s="5"/>
-      <c r="B67" s="17" t="s">
+      <c r="B67" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C67" s="18"/>
-      <c r="D67" s="18"/>
-      <c r="E67" s="18"/>
-      <c r="F67" s="18"/>
-      <c r="G67" s="18"/>
-      <c r="H67" s="18"/>
-      <c r="I67" s="18"/>
-      <c r="J67" s="18"/>
-      <c r="K67" s="18"/>
-      <c r="L67" s="18"/>
-      <c r="M67" s="18"/>
-      <c r="N67" s="19"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="17"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="17"/>
+      <c r="J67" s="17"/>
+      <c r="K67" s="17"/>
+      <c r="L67" s="17"/>
+      <c r="M67" s="17"/>
+      <c r="N67" s="18"/>
       <c r="O67" s="10"/>
     </row>
     <row r="68" spans="1:15" ht="27" hidden="1" customHeight="1">
@@ -3912,7 +3912,7 @@
         <v>0.8571428571428571</v>
       </c>
       <c r="J70" s="6">
-        <f t="shared" ref="J70:O70" si="31">SUM(J68:J69)</f>
+        <f t="shared" ref="J70:O70" si="33">SUM(J68:J69)</f>
         <v>14640</v>
       </c>
       <c r="K70" s="13">
@@ -3920,40 +3920,40 @@
         <v>0.35269459635259826</v>
       </c>
       <c r="L70" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>13152</v>
       </c>
       <c r="M70" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="N70" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>96</v>
       </c>
       <c r="O70" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:15" ht="27" customHeight="1">
       <c r="A71" s="5"/>
-      <c r="B71" s="16" t="s">
+      <c r="B71" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C71" s="16"/>
-      <c r="D71" s="16"/>
-      <c r="E71" s="16"/>
-      <c r="F71" s="16"/>
-      <c r="G71" s="16"/>
-      <c r="H71" s="16"/>
-      <c r="I71" s="16"/>
-      <c r="J71" s="16"/>
-      <c r="K71" s="16"/>
-      <c r="L71" s="16"/>
-      <c r="M71" s="16"/>
-      <c r="N71" s="16"/>
-      <c r="O71" s="16"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="19"/>
+      <c r="G71" s="19"/>
+      <c r="H71" s="19"/>
+      <c r="I71" s="19"/>
+      <c r="J71" s="19"/>
+      <c r="K71" s="19"/>
+      <c r="L71" s="19"/>
+      <c r="M71" s="19"/>
+      <c r="N71" s="19"/>
+      <c r="O71" s="19"/>
     </row>
     <row r="72" spans="1:15" ht="27" customHeight="1">
       <c r="A72" s="5"/>
@@ -3976,7 +3976,7 @@
         <v>72</v>
       </c>
       <c r="I72" s="13">
-        <f>H72/H$81</f>
+        <f t="shared" ref="I72:I77" si="34">H72/H$81</f>
         <v>0.6428571428571429</v>
       </c>
       <c r="J72" s="6">
@@ -3984,7 +3984,7 @@
         <v>10980</v>
       </c>
       <c r="K72" s="13">
-        <f>J72/J$81</f>
+        <f t="shared" ref="K72:K77" si="35">J72/J$81</f>
         <v>0.26452094726444869</v>
       </c>
       <c r="L72" s="6">
@@ -4023,7 +4023,7 @@
         <v>0</v>
       </c>
       <c r="I73" s="13">
-        <f>H73/H$81</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="J73" s="6">
@@ -4031,7 +4031,7 @@
         <v>66</v>
       </c>
       <c r="K73" s="13">
-        <f>J73/J$81</f>
+        <f t="shared" si="35"/>
         <v>1.5900166229010576E-3</v>
       </c>
       <c r="L73" s="6">
@@ -4064,7 +4064,7 @@
         <v>50</v>
       </c>
       <c r="I74" s="13">
-        <f>H74/H$81</f>
+        <f t="shared" si="34"/>
         <v>0.44642857142857145</v>
       </c>
       <c r="J74" s="6">
@@ -4072,7 +4072,7 @@
         <v>10929</v>
       </c>
       <c r="K74" s="13">
-        <f>J74/J$81</f>
+        <f t="shared" si="35"/>
         <v>0.26329229805584331</v>
       </c>
       <c r="L74" s="6">
@@ -4105,7 +4105,7 @@
         <v>18</v>
       </c>
       <c r="I75" s="13">
-        <f>H75/H$81</f>
+        <f t="shared" si="34"/>
         <v>0.16071428571428573</v>
       </c>
       <c r="J75" s="6">
@@ -4113,7 +4113,7 @@
         <v>6564</v>
       </c>
       <c r="K75" s="13">
-        <f>J75/J$81</f>
+        <f t="shared" si="35"/>
         <v>0.15813438049579609</v>
       </c>
       <c r="L75" s="6">
@@ -4146,7 +4146,7 @@
         <v>12</v>
       </c>
       <c r="I76" s="13">
-        <f>H76/H$81</f>
+        <f t="shared" si="34"/>
         <v>0.10714285714285714</v>
       </c>
       <c r="J76" s="6">
@@ -4154,7 +4154,7 @@
         <v>1830</v>
       </c>
       <c r="K76" s="13">
-        <f>J76/J$81</f>
+        <f t="shared" si="35"/>
         <v>4.4086824544074782E-2</v>
       </c>
       <c r="L76" s="6">
@@ -4198,7 +4198,7 @@
         <v>152</v>
       </c>
       <c r="I77" s="13">
-        <f>H77/H$81</f>
+        <f t="shared" si="34"/>
         <v>1.3571428571428572</v>
       </c>
       <c r="J77" s="6">
@@ -4206,44 +4206,44 @@
         <v>30369</v>
       </c>
       <c r="K77" s="13">
-        <f>J77/J$81</f>
+        <f t="shared" si="35"/>
         <v>0.73162446698306394</v>
       </c>
       <c r="L77" s="6">
-        <f t="shared" ref="J77:O77" si="32">SUM(L72:L76)</f>
+        <f t="shared" ref="L77:O77" si="36">SUM(L72:L76)</f>
         <v>20824</v>
       </c>
       <c r="M77" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="N77" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>152</v>
       </c>
       <c r="O77" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:15" ht="27" customHeight="1">
       <c r="A78" s="5"/>
-      <c r="B78" s="16" t="s">
+      <c r="B78" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C78" s="16"/>
-      <c r="D78" s="16"/>
-      <c r="E78" s="16"/>
-      <c r="F78" s="16"/>
-      <c r="G78" s="16"/>
-      <c r="H78" s="16"/>
-      <c r="I78" s="16"/>
-      <c r="J78" s="16"/>
-      <c r="K78" s="16"/>
-      <c r="L78" s="16"/>
-      <c r="M78" s="16"/>
-      <c r="N78" s="16"/>
-      <c r="O78" s="16"/>
+      <c r="C78" s="19"/>
+      <c r="D78" s="19"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="19"/>
+      <c r="G78" s="19"/>
+      <c r="H78" s="19"/>
+      <c r="I78" s="19"/>
+      <c r="J78" s="19"/>
+      <c r="K78" s="19"/>
+      <c r="L78" s="19"/>
+      <c r="M78" s="19"/>
+      <c r="N78" s="19"/>
+      <c r="O78" s="19"/>
     </row>
     <row r="79" spans="1:15" ht="27" customHeight="1">
       <c r="A79" s="5"/>
@@ -4263,47 +4263,47 @@
       </c>
       <c r="J79" s="6">
         <f>SUM(J77+J66+J62)</f>
-        <v>41779</v>
+        <v>42955</v>
       </c>
       <c r="K79" s="13">
         <f>J79/J$81</f>
-        <v>1.0065046134573226</v>
+        <v>1.034835818738105</v>
       </c>
       <c r="L79" s="6">
-        <f t="shared" ref="L79:O79" si="33">SUM(L77+L66+L62)</f>
-        <v>31292</v>
+        <f t="shared" ref="L79:O79" si="37">SUM(L77+L66+L62)</f>
+        <v>32388</v>
       </c>
       <c r="M79" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="N79" s="6">
         <f>SUM(N77+N66+N62)</f>
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="O79" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:15" ht="27" customHeight="1">
       <c r="A80" s="5"/>
-      <c r="B80" s="16" t="s">
+      <c r="B80" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C80" s="16"/>
-      <c r="D80" s="16"/>
-      <c r="E80" s="16"/>
-      <c r="F80" s="16"/>
-      <c r="G80" s="16"/>
-      <c r="H80" s="16"/>
-      <c r="I80" s="16"/>
-      <c r="J80" s="16"/>
-      <c r="K80" s="16"/>
-      <c r="L80" s="16"/>
-      <c r="M80" s="16"/>
-      <c r="N80" s="16"/>
-      <c r="O80" s="16"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="19"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="19"/>
+      <c r="G80" s="19"/>
+      <c r="H80" s="19"/>
+      <c r="I80" s="19"/>
+      <c r="J80" s="19"/>
+      <c r="K80" s="19"/>
+      <c r="L80" s="19"/>
+      <c r="M80" s="19"/>
+      <c r="N80" s="19"/>
+      <c r="O80" s="19"/>
     </row>
     <row r="81" spans="1:15" ht="27" customHeight="1">
       <c r="A81" s="5"/>
@@ -4359,7 +4359,7 @@
     </row>
     <row r="85" spans="1:15" ht="27" customHeight="1">
       <c r="B85" s="7">
-        <v>4.0000000000000003E-5</v>
+        <v>3.9999999999999998E-6</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>43</v>
@@ -4368,7 +4368,7 @@
     <row r="86" spans="1:15" ht="27" customHeight="1">
       <c r="B86" s="7">
         <f>B85/B84</f>
-        <v>1000.0000000000001</v>
+        <v>100</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>44</v>
@@ -4394,6 +4394,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B20:N20"/>
     <mergeCell ref="B46:N46"/>
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="B51:O51"/>
@@ -4410,7 +4411,6 @@
     <mergeCell ref="B40:O40"/>
     <mergeCell ref="B55:N55"/>
     <mergeCell ref="B67:N67"/>
-    <mergeCell ref="B20:N20"/>
   </mergeCells>
   <conditionalFormatting sqref="I51:I54 I1:I5 I7:I19 I56:I66 I21:I39 I68:I1048576">
     <cfRule type="colorScale" priority="35">

</xml_diff>

<commit_message>
Updated sine and cosine estimation.
</commit_message>
<xml_diff>
--- a/doc/design/bill_of_materials.xlsx
+++ b/doc/design/bill_of_materials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -993,8 +993,8 @@
   <dimension ref="A1:O91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B85" sqref="B85"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24:O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0"/>
@@ -1667,7 +1667,7 @@
         <v>31</v>
       </c>
       <c r="C16" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>24</v>
@@ -1687,15 +1687,15 @@
       </c>
       <c r="J16" s="6">
         <f>$C16*J$4</f>
-        <v>292</v>
+        <v>438</v>
       </c>
       <c r="K16" s="13">
         <f>J16/J$81</f>
-        <v>7.0346189982895277E-3</v>
+        <v>1.0551928497434292E-2</v>
       </c>
       <c r="L16" s="6">
         <f>$C16*L$4</f>
-        <v>302</v>
+        <v>453</v>
       </c>
       <c r="M16" s="6">
         <f t="shared" ref="M16:O16" si="2">$C16*M$4</f>
@@ -1716,7 +1716,7 @@
         <v>30</v>
       </c>
       <c r="C17" s="6">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>24</v>
@@ -1728,23 +1728,23 @@
       <c r="G17" s="6"/>
       <c r="H17" s="6">
         <f>$C17*H$5</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="I17" s="13">
         <f>H17/H$81</f>
-        <v>3.5714285714285712E-2</v>
+        <v>0.125</v>
       </c>
       <c r="J17" s="6">
         <f t="shared" ref="J17:O18" si="3">$C17*J$5</f>
-        <v>588</v>
+        <v>2058</v>
       </c>
       <c r="K17" s="13">
         <f>J17/J$81</f>
-        <v>1.4165602640391241E-2</v>
+        <v>4.9579609241369345E-2</v>
       </c>
       <c r="L17" s="6">
         <f t="shared" si="3"/>
-        <v>548</v>
+        <v>1918</v>
       </c>
       <c r="M17" s="6">
         <f t="shared" si="3"/>
@@ -1752,7 +1752,7 @@
       </c>
       <c r="N17" s="6">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="O17" s="6">
         <f t="shared" si="3"/>
@@ -1765,7 +1765,7 @@
         <v>29</v>
       </c>
       <c r="C18" s="6">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>24</v>
@@ -1777,23 +1777,23 @@
       <c r="G18" s="6"/>
       <c r="H18" s="6">
         <f>$C18*H$5</f>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="I18" s="13">
         <f>H18/H$81</f>
-        <v>7.1428571428571425E-2</v>
+        <v>0.17857142857142858</v>
       </c>
       <c r="J18" s="6">
         <f>$C18*J$5</f>
-        <v>1176</v>
+        <v>2940</v>
       </c>
       <c r="K18" s="13">
         <f>J18/J$81</f>
-        <v>2.8331205280782482E-2</v>
+        <v>7.0828013201956197E-2</v>
       </c>
       <c r="L18" s="6">
         <f>$C18*L$5</f>
-        <v>1096</v>
+        <v>2740</v>
       </c>
       <c r="M18" s="6">
         <f t="shared" si="3"/>
@@ -1801,7 +1801,7 @@
       </c>
       <c r="N18" s="6">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="O18" s="6">
         <f t="shared" si="3"/>
@@ -1823,29 +1823,29 @@
         <v>25</v>
       </c>
       <c r="F19" s="6">
-        <f>2*F4+2*F5+F3</f>
-        <v>14</v>
+        <f>3*F4+3*F5+F3</f>
+        <v>20</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6">
         <f>SUM(H16:H18)</f>
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="I19" s="13">
         <f>H19/H$81</f>
-        <v>0.10714285714285714</v>
+        <v>0.30357142857142855</v>
       </c>
       <c r="J19" s="6">
         <f t="shared" ref="J19:O19" si="4">SUM(J16:J18)</f>
-        <v>2056</v>
+        <v>5436</v>
       </c>
       <c r="K19" s="13">
         <f>J19/J$81</f>
-        <v>4.9531426919463252E-2</v>
+        <v>0.13095955094075984</v>
       </c>
       <c r="L19" s="6">
         <f t="shared" si="4"/>
-        <v>1946</v>
+        <v>5111</v>
       </c>
       <c r="M19" s="6">
         <f t="shared" si="4"/>
@@ -1853,7 +1853,7 @@
       </c>
       <c r="N19" s="6">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="O19" s="6">
         <f t="shared" si="4"/>
@@ -3163,23 +3163,23 @@
       <c r="G52" s="6"/>
       <c r="H52" s="6">
         <f>$C52*H19</f>
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="I52" s="13">
         <f>H52/H$81</f>
-        <v>0.21428571428571427</v>
+        <v>0.6071428571428571</v>
       </c>
       <c r="J52" s="6">
         <f>$C52*J19</f>
-        <v>4112</v>
+        <v>10872</v>
       </c>
       <c r="K52" s="13">
         <f>J52/J$81</f>
-        <v>9.9062853838926504E-2</v>
+        <v>0.26191910188151968</v>
       </c>
       <c r="L52" s="6">
         <f>$C52*L19</f>
-        <v>3892</v>
+        <v>10222</v>
       </c>
       <c r="M52" s="6">
         <f>$C52*M19</f>
@@ -3187,7 +3187,7 @@
       </c>
       <c r="N52" s="6">
         <f>$C52*N19</f>
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="O52" s="6">
         <f>$C52*O19</f>
@@ -3253,28 +3253,28 @@
       <c r="E54" s="6"/>
       <c r="F54" s="6">
         <f>1*F19+1*F5</f>
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G54" s="6"/>
       <c r="H54" s="6">
         <f>SUM(H52:H53)</f>
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="I54" s="13">
         <f>H54/H$81</f>
-        <v>0.32142857142857145</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="J54" s="6">
         <f t="shared" ref="J54:O54" si="27">SUM(J52:J53)</f>
-        <v>5876</v>
+        <v>12636</v>
       </c>
       <c r="K54" s="13">
         <f>J54/J$81</f>
-        <v>0.14155966176010021</v>
+        <v>0.3044159098026934</v>
       </c>
       <c r="L54" s="6">
         <f t="shared" si="27"/>
-        <v>5536</v>
+        <v>11866</v>
       </c>
       <c r="M54" s="6">
         <f t="shared" si="27"/>
@@ -3282,7 +3282,7 @@
       </c>
       <c r="N54" s="6">
         <f t="shared" si="27"/>
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="O54" s="6">
         <f t="shared" si="27"/>
@@ -3375,23 +3375,23 @@
       <c r="G57" s="6"/>
       <c r="H57" s="6">
         <f>$C57*H54</f>
-        <v>108</v>
+        <v>240</v>
       </c>
       <c r="I57" s="13">
         <f>H57/H$81</f>
-        <v>0.9642857142857143</v>
+        <v>2.1428571428571428</v>
       </c>
       <c r="J57" s="6">
         <f t="shared" ref="J57:N57" si="28">$C57*J54</f>
-        <v>17628</v>
+        <v>37908</v>
       </c>
       <c r="K57" s="13">
         <f>J57/J$81</f>
-        <v>0.42467898528030068</v>
+        <v>0.91324772940808019</v>
       </c>
       <c r="L57" s="6">
         <f t="shared" si="28"/>
-        <v>16608</v>
+        <v>35598</v>
       </c>
       <c r="M57" s="6">
         <f t="shared" si="28"/>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="N57" s="6">
         <f t="shared" si="28"/>
-        <v>108</v>
+        <v>240</v>
       </c>
       <c r="O57" s="6">
         <f>$C57*O54</f>
@@ -3418,23 +3418,23 @@
       <c r="G58" s="6"/>
       <c r="H58" s="6">
         <f>SUM(H56:H57)</f>
-        <v>172</v>
+        <v>304</v>
       </c>
       <c r="I58" s="13">
         <f>H58/H$81</f>
-        <v>1.5357142857142858</v>
+        <v>2.7142857142857144</v>
       </c>
       <c r="J58" s="6">
         <f t="shared" ref="J58:O58" si="29">SUM(J56:J57)</f>
-        <v>27388</v>
+        <v>47668</v>
       </c>
       <c r="K58" s="13">
         <f>J58/J$81</f>
-        <v>0.65980871618203285</v>
+        <v>1.1483774603098122</v>
       </c>
       <c r="L58" s="6">
         <f t="shared" si="29"/>
-        <v>25376</v>
+        <v>44366</v>
       </c>
       <c r="M58" s="6">
         <f t="shared" si="29"/>
@@ -3442,7 +3442,7 @@
       </c>
       <c r="N58" s="6">
         <f t="shared" si="29"/>
-        <v>172</v>
+        <v>304</v>
       </c>
       <c r="O58" s="6">
         <f t="shared" si="29"/>
@@ -3486,23 +3486,23 @@
       <c r="G60" s="6"/>
       <c r="H60" s="6">
         <f>$C60*H52</f>
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="I60" s="13">
         <f>H60/H$81</f>
-        <v>0.21428571428571427</v>
+        <v>0.6071428571428571</v>
       </c>
       <c r="J60" s="6">
         <f>$C60*J54</f>
-        <v>5876</v>
+        <v>12636</v>
       </c>
       <c r="K60" s="13">
         <f>J60/J$81</f>
-        <v>0.14155966176010021</v>
+        <v>0.3044159098026934</v>
       </c>
       <c r="L60" s="6">
         <f t="shared" ref="L60:O60" si="30">$C60*L54</f>
-        <v>5536</v>
+        <v>11866</v>
       </c>
       <c r="M60" s="6">
         <f t="shared" si="30"/>
@@ -3510,7 +3510,7 @@
       </c>
       <c r="N60" s="6">
         <f t="shared" si="30"/>
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="O60" s="6">
         <f t="shared" si="30"/>
@@ -3576,7 +3576,7 @@
       <c r="E62" s="6"/>
       <c r="F62" s="6">
         <f>6*F54+1*F27</f>
-        <v>116</v>
+        <v>152</v>
       </c>
       <c r="G62" s="6"/>
       <c r="H62" s="6">
@@ -3589,15 +3589,15 @@
       </c>
       <c r="J62" s="6">
         <f>SUM(J60:J61)</f>
-        <v>10756</v>
+        <v>17516</v>
       </c>
       <c r="K62" s="13">
         <f>J62/J$81</f>
-        <v>0.25912452721096629</v>
+        <v>0.42198077525355948</v>
       </c>
       <c r="L62" s="6">
         <f t="shared" ref="L62:O62" si="31">SUM(L60:L61)</f>
-        <v>9920</v>
+        <v>16250</v>
       </c>
       <c r="M62" s="6">
         <f t="shared" si="31"/>
@@ -3605,7 +3605,7 @@
       </c>
       <c r="N62" s="6">
         <f t="shared" si="31"/>
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="O62" s="6">
         <f t="shared" si="31"/>
@@ -4263,15 +4263,15 @@
       </c>
       <c r="J79" s="6">
         <f>SUM(J77+J66+J62)</f>
-        <v>42955</v>
+        <v>49715</v>
       </c>
       <c r="K79" s="13">
         <f>J79/J$81</f>
-        <v>1.034835818738105</v>
+        <v>1.1976920667806981</v>
       </c>
       <c r="L79" s="6">
         <f t="shared" ref="L79:O79" si="37">SUM(L77+L66+L62)</f>
-        <v>32388</v>
+        <v>38718</v>
       </c>
       <c r="M79" s="6">
         <f t="shared" si="37"/>
@@ -4279,7 +4279,7 @@
       </c>
       <c r="N79" s="6">
         <f>SUM(N77+N66+N62)</f>
-        <v>232</v>
+        <v>276</v>
       </c>
       <c r="O79" s="6">
         <f t="shared" si="37"/>
@@ -4394,11 +4394,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B20:N20"/>
-    <mergeCell ref="B46:N46"/>
-    <mergeCell ref="B2:O2"/>
-    <mergeCell ref="B51:O51"/>
-    <mergeCell ref="B59:O59"/>
     <mergeCell ref="B80:O80"/>
     <mergeCell ref="B71:O71"/>
     <mergeCell ref="B15:O15"/>
@@ -4411,6 +4406,11 @@
     <mergeCell ref="B40:O40"/>
     <mergeCell ref="B55:N55"/>
     <mergeCell ref="B67:N67"/>
+    <mergeCell ref="B20:N20"/>
+    <mergeCell ref="B46:N46"/>
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B51:O51"/>
+    <mergeCell ref="B59:O59"/>
   </mergeCells>
   <conditionalFormatting sqref="I51:I54 I1:I5 I7:I19 I56:I66 I21:I39 I68:I1048576">
     <cfRule type="colorScale" priority="35">

</xml_diff>